<commit_message>
Test case number 4 is passing without progressive aggregation. Building the test cases for cleaning a multicolumn time index, which is the new challenge in test case number 5.
</commit_message>
<xml_diff>
--- a/tests/integration_cases/expected/test_case4.xlsx
+++ b/tests/integration_cases/expected/test_case4.xlsx
@@ -16,28 +16,28 @@
     <t>datetime</t>
   </si>
   <si>
-    <t>Mercado de trabajo - EPH -Evolucion de la situacion ocupacional 1 -Tasas (31 aglomerados relevados) -Actividad</t>
+    <t>Actividad</t>
   </si>
   <si>
-    <t>Mercado de trabajo - EPH -Evolucion de la situacion ocupacional 1 -Tasas (31 aglomerados relevados) -Empleo</t>
+    <t>Empleo</t>
   </si>
   <si>
-    <t>Mercado de trabajo - EPH -Evolucion de la situacion ocupacional 1 -Tasas (31 aglomerados relevados) -Desocupacion</t>
+    <t>Desocupacion</t>
   </si>
   <si>
-    <t>Mercado de trabajo - EPH -Evolucion de la situacion ocupacional 1 -Tasas (31 aglomerados relevados) -Subocupacion</t>
+    <t>Subocupacion</t>
   </si>
   <si>
-    <t>Poblacion (Total urbano 3 - en miles de personas) -Poblacion total</t>
+    <t>Poblacion total</t>
   </si>
   <si>
-    <t>Poblacion (Total urbano 3 - en miles de personas) -PEA</t>
+    <t>PEA</t>
   </si>
   <si>
-    <t>Poblacion (Total urbano 3 - en miles de personas) -Ocupados</t>
+    <t>Ocupados</t>
   </si>
   <si>
-    <t>Poblacion (Total urbano 3 - en miles de personas) -Desocupados</t>
+    <t>Desocupados</t>
   </si>
 </sst>
 </file>
@@ -47,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -59,12 +59,17 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -111,15 +116,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>

</xml_diff>